<commit_message>
updated and refactored code
</commit_message>
<xml_diff>
--- a/src/main/resources/rules/sljournalentryrules.xlsx
+++ b/src/main/resources/rules/sljournalentryrules.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sv864cc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sv864cc\Desktop\GM\Drools\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="90">
   <si>
     <t>RuleSet</t>
   </si>
@@ -95,6 +95,195 @@
     <t>Acctng Treatment ID</t>
   </si>
   <si>
+    <t>LOAN_RGLR_PMT and PRNCPL_PMT with Amt &gt; 0</t>
+  </si>
+  <si>
+    <t>LOAN_RGLR_PMT and PRNCPL_PMT with Amt &lt; 0</t>
+  </si>
+  <si>
+    <t>"1350921-01"</t>
+  </si>
+  <si>
+    <t>"1350210-01"</t>
+  </si>
+  <si>
+    <t>"DR"</t>
+  </si>
+  <si>
+    <t>"GAAP"</t>
+  </si>
+  <si>
+    <t>"CR"</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>"UPBP_01"</t>
+  </si>
+  <si>
+    <t>$pesign:PostingEventWithAmountSign</t>
+  </si>
+  <si>
+    <t>PostingRuleSetCode</t>
+  </si>
+  <si>
+    <t>amtSignCd</t>
+  </si>
+  <si>
+    <t>P: Positive; N: Negative</t>
+  </si>
+  <si>
+    <t>LOAN_SLE</t>
+  </si>
+  <si>
+    <t>PRNCPL_RLF_CSH_SS</t>
+  </si>
+  <si>
+    <t>"UPBRCS_01"</t>
+  </si>
+  <si>
+    <t>"1350932-01"</t>
+  </si>
+  <si>
+    <t>LOAN_SLE and PRNCPL_RLF_CSH_SS with Amt &gt; 0</t>
+  </si>
+  <si>
+    <t>LOAN_SLE and PRNCPL_RLF_CSH_SS with Amt &lt; 0</t>
+  </si>
+  <si>
+    <t>ESCRW_DPST</t>
+  </si>
+  <si>
+    <t>"EDD_01"</t>
+  </si>
+  <si>
+    <t>"AIRP_01"</t>
+  </si>
+  <si>
+    <t>"AIRP_02"</t>
+  </si>
+  <si>
+    <t>"9999999-01"</t>
+  </si>
+  <si>
+    <t>"9999999-02"</t>
+  </si>
+  <si>
+    <t>"9999999-03"</t>
+  </si>
+  <si>
+    <t>"1340921-01"</t>
+  </si>
+  <si>
+    <t>"1340210-01"</t>
+  </si>
+  <si>
+    <t>"1340210-02"</t>
+  </si>
+  <si>
+    <t>INTRST_PMT</t>
+  </si>
+  <si>
+    <t>UNPPLD_SSPNS_FNDS</t>
+  </si>
+  <si>
+    <t>"MAUC_01"</t>
+  </si>
+  <si>
+    <t>"9999999-04"</t>
+  </si>
+  <si>
+    <t>CORP_ADV_ADJSTMNT_RLF_ALLWNC</t>
+  </si>
+  <si>
+    <t>"CAARACO_01"</t>
+  </si>
+  <si>
+    <t>"1310411-02"</t>
+  </si>
+  <si>
+    <t>"1359210-01"</t>
+  </si>
+  <si>
+    <t>"CAARACO_02"</t>
+  </si>
+  <si>
+    <t>"1359211-01"</t>
+  </si>
+  <si>
+    <t>TI_ADV_ADJSTMNT_RLF_ALLWNC</t>
+  </si>
+  <si>
+    <t>"TIARACO_01"</t>
+  </si>
+  <si>
+    <t>"1310211-02"</t>
+  </si>
+  <si>
+    <t>"1359210-02"</t>
+  </si>
+  <si>
+    <t>LOAN_RGLR_PMT and ESCRW_DPST with Amt &gt; 0</t>
+  </si>
+  <si>
+    <t>LOAN_RGLR_PMT and UNPPLD_SSPNS_FNDS with Amt &gt; 0</t>
+  </si>
+  <si>
+    <t>LOAN_RGLR_PMT and CORP_ADV_ADJSTMNT_RLF_ALLWNC with Amt &gt; 0</t>
+  </si>
+  <si>
+    <t>LOAN_RGLR_PMT and ESCRW_DPST with Amt &lt; 0</t>
+  </si>
+  <si>
+    <t>LOAN_RGLR_PMT and INTRST_PMT with Amt &gt; 0</t>
+  </si>
+  <si>
+    <t>LOAN_RGLR_PMT and INTRST_PMT with Amt &lt; 0</t>
+  </si>
+  <si>
+    <t>LOAN_RGLR_PMT and UNPPLD_SSPNS_FNDS with Amt &lt; 0</t>
+  </si>
+  <si>
+    <t>LOAN_RGLR_PMT and CORP_ADV_ADJSTMNT_RLF_ALLWNC with Amt &lt; 0</t>
+  </si>
+  <si>
+    <t>LOAN_RGLR_PMT and TI_ADV_ADJSTMNT_RLF_ALLWNC with Amt &gt; 0</t>
+  </si>
+  <si>
+    <t>LOAN_RGLR_PMT and TI_ADV_ADJSTMNT_RLF_ALLWNC with Amt &lt; 0</t>
+  </si>
+  <si>
+    <t>slje.setPstngRuleSetCd($param);</t>
+  </si>
+  <si>
+    <t>SLJournalEntry slje</t>
+  </si>
+  <si>
+    <t>slje.setDrSLAcctNm($param);</t>
+  </si>
+  <si>
+    <t>slje.setDrDbOrCrCd($param);</t>
+  </si>
+  <si>
+    <t>slje.setDrAcctngBasisCd($param);</t>
+  </si>
+  <si>
+    <t>slje.setCrSLAcctNm($param);</t>
+  </si>
+  <si>
+    <t>slje.setCrDbOrCrCd($param);</t>
+  </si>
+  <si>
+    <t>slje.setCrAcctngBasisCd($param);</t>
+  </si>
+  <si>
+    <t>com.sample.SLdroolsspringboot.SLPostingEvent, com.sample.SLdroolsspringboot.SLJournalEntry, com.sample.SLdroolsspringboot.PostingEventWithAmountSign</t>
+  </si>
+  <si>
     <t>trnType</t>
   </si>
   <si>
@@ -105,75 +294,6 @@
   </si>
   <si>
     <t>insuredInd</t>
-  </si>
-  <si>
-    <t>setDrSLAcctNm($param);</t>
-  </si>
-  <si>
-    <t>setDrDbOrCrCd($param);</t>
-  </si>
-  <si>
-    <t>setDrAcctngBasisCd($param);</t>
-  </si>
-  <si>
-    <t>setCrSLAcctNm($param);</t>
-  </si>
-  <si>
-    <t>setCrDbOrCrCd($param);</t>
-  </si>
-  <si>
-    <t>setCrAcctngBasisCd($param);</t>
-  </si>
-  <si>
-    <t>LOAN_RGLR_PMT and PRNCPL_PMT with Amt &gt; 0</t>
-  </si>
-  <si>
-    <t>LOAN_RGLR_PMT and PRNCPL_PMT with Amt &lt; 0</t>
-  </si>
-  <si>
-    <t>"1350921-01"</t>
-  </si>
-  <si>
-    <t>"1350210-01"</t>
-  </si>
-  <si>
-    <t>"DR"</t>
-  </si>
-  <si>
-    <t>"GAAP"</t>
-  </si>
-  <si>
-    <t>"CR"</t>
-  </si>
-  <si>
-    <t>$slje:SLJournalEntry</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>"UPBP_01"</t>
-  </si>
-  <si>
-    <t>setPstngRuleSetCd($param);</t>
-  </si>
-  <si>
-    <t>$pesign:PostingEventWithAmountSign</t>
-  </si>
-  <si>
-    <t>PostingRuleSetCode</t>
-  </si>
-  <si>
-    <t>com.sample.SLdroolsspringboot.SLPostingEvent, com.sample.SLdroolsspringboot.SLJournalEntry, util.OutputFormat, com.sample.SLdroolsspringboot.PostingEventWithAmountSign</t>
-  </si>
-  <si>
-    <t>amtSignCd</t>
-  </si>
-  <si>
-    <t>P: Positive; N: Negative</t>
   </si>
 </sst>
 </file>
@@ -293,7 +413,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -312,8 +432,12 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -635,17 +759,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.21875" customWidth="1"/>
+    <col min="1" max="1" width="52.44140625" customWidth="1"/>
     <col min="2" max="2" width="16.88671875" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="29.6640625" customWidth="1"/>
     <col min="4" max="4" width="19.5546875" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="16.44140625" style="9" customWidth="1"/>
@@ -655,7 +779,7 @@
     <col min="10" max="10" width="25.33203125" customWidth="1"/>
     <col min="11" max="11" width="23" customWidth="1"/>
     <col min="12" max="12" width="21.6640625" customWidth="1"/>
-    <col min="13" max="13" width="25.109375" customWidth="1"/>
+    <col min="13" max="13" width="28.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -671,14 +795,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>47</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
@@ -748,60 +874,58 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
-      <c r="B8" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="18"/>
+      <c r="B8" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="19"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="5" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>24</v>
+        <v>87</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>25</v>
+        <v>88</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>26</v>
+        <v>89</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -819,10 +943,10 @@
         <v>11</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>13</v>
@@ -845,7 +969,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>7</v>
@@ -860,33 +984,33 @@
         <v>9</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>7</v>
@@ -901,34 +1025,771 @@
         <v>9</v>
       </c>
       <c r="F12" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="K13" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="L13" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="M13" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="B14" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="13">
+        <v>1</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J14" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="K14" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="M14" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="H12" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="J12" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="K12" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>38</v>
+      <c r="D15" s="13">
+        <v>2</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J15" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="K15" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="L15" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="M15" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="13">
+        <v>2</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J16" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="K16" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="L16" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="M16" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="13">
+        <v>1</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J17" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="K17" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="L17" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="M17" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="13">
+        <v>1</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J18" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="K18" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="L18" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="M18" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="13">
+        <v>5</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J19" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="K19" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="L19" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="M19" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="13">
+        <v>5</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J20" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="K20" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="L20" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="M20" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="13">
+        <v>6</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J21" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="K21" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="L21" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="M21" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="13">
+        <v>6</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J22" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="K22" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="L22" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="M22" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="13">
+        <v>1</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J23" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="K23" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="L23" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="M23" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="13">
+        <v>1</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J24" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="K24" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="L24" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="M24" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="13">
+        <v>5</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J25" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="K25" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="L25" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="M25" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="13">
+        <v>5</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J26" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="K26" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="L26" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="M26" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="13">
+        <v>5</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="I27" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J27" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="K27" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="L27" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="M27" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="13">
+        <v>5</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="I28" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J28" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="K28" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="L28" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="M28" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="13">
+        <v>1</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J29" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="K29" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="L29" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="M29" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="13">
+        <v>1</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J30" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="K30" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="L30" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="M30" s="13" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="B8:F8"/>
-    <mergeCell ref="G8:M8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>